<commit_message>
More polished grade set.
</commit_message>
<xml_diff>
--- a/mymaterial/Semester2/grades/homework_and_reading.xlsx
+++ b/mymaterial/Semester2/grades/homework_and_reading.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="72" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="74" xml:space="preserve">
   <si>
     <t>Tutor Student Scores</t>
   </si>
@@ -21,7 +21,7 @@
     <t>PHYS135B</t>
   </si>
   <si>
-    <t>Exported 04/02/2021</t>
+    <t>Exported 04/12/2021</t>
   </si>
   <si>
     <t>1st</t>
@@ -30,6 +30,9 @@
     <t>Averages</t>
   </si>
   <si>
+    <t>Homework 5</t>
+  </si>
+  <si>
     <t>Homework 4</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
   </si>
   <si>
     <t>First Assignment (Testing)</t>
+  </si>
+  <si>
+    <t>Due 4/2/2021</t>
   </si>
   <si>
     <t>Due 3/28/2021</t>
@@ -1111,6 +1117,8 @@
     <col min="26" max="26" bestFit="1" customWidth="1" width="16"/>
     <col min="27" max="27" bestFit="1" customWidth="1" width="16"/>
     <col min="28" max="28" bestFit="1" customWidth="1" width="16"/>
+    <col min="29" max="29" bestFit="1" customWidth="1" width="16"/>
+    <col min="30" max="30" bestFit="1" customWidth="1" width="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1209,6 +1217,9 @@
       <c r="Q7" s="10" t="s">
         <v>15</v>
       </c>
+      <c r="R7" s="10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="8">
       <c r="A8" s="0" t="inlineStr">
@@ -1242,37 +1253,40 @@
         </is>
       </c>
       <c r="G8" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P8" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="9">
@@ -1292,57 +1306,60 @@
         </is>
       </c>
       <c r="D9" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="R9" s="15" t="s">
+        <v>30</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="10">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" s="12" t="inlineStr">
         <is>
@@ -1414,7 +1431,7 @@
           <t/>
         </is>
       </c>
-      <c r="R10" s="0" t="inlineStr">
+      <c r="R10" s="15" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -1465,6 +1482,16 @@
         </is>
       </c>
       <c r="AB10" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC10" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD10" s="0" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -1472,10 +1499,10 @@
     </row>
     <row customHeight="1" ht="15" r="11">
       <c r="A11" s="18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="23" t="inlineStr">
         <is>
@@ -1486,51 +1513,54 @@
         <f>IFERROR(SUM(0.5*E11,0.5*F11),0)</f>
       </c>
       <c r="E11" s="26" t="str">
-        <f>IFERROR(AVERAGE(G11,J11,M11,O11),0)</f>
+        <f>IFERROR(AVERAGE(G11,H11,K11,N11,P11),0)</f>
       </c>
       <c r="F11" s="26" t="str">
-        <f>IFERROR(AVERAGE(H11,I11,K11,L11,N11,P11,Q11),0)</f>
+        <f>IFERROR(AVERAGE(I11,J11,L11,M11,O11,Q11,R11),0)</f>
       </c>
       <c r="G11" s="25" t="n">
         <v>1.0</v>
       </c>
       <c r="H11" s="25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I11" s="25" t="n">
         <v>0.9454545454545454</v>
       </c>
-      <c r="I11" s="25" t="n">
+      <c r="J11" s="25" t="n">
         <v>0.97</v>
       </c>
-      <c r="J11" s="25" t="n">
+      <c r="K11" s="25" t="n">
         <v>0.7272727272727273</v>
       </c>
-      <c r="K11" s="25" t="n">
+      <c r="L11" s="25" t="n">
         <v>0.9600000000000001</v>
       </c>
-      <c r="L11" s="25" t="n">
+      <c r="M11" s="25" t="n">
         <v>0.975</v>
       </c>
-      <c r="M11" s="25" t="n">
+      <c r="N11" s="25" t="n">
         <v>0.6875</v>
       </c>
-      <c r="N11" s="25" t="n">
+      <c r="O11" s="25" t="n">
         <v>0.9874999999999999</v>
       </c>
-      <c r="O11" s="25" t="n">
+      <c r="P11" s="25" t="n">
         <v>0.8125</v>
       </c>
-      <c r="P11" s="25" t="n">
+      <c r="Q11" s="25" t="n">
         <v>0.9684210526315788</v>
       </c>
-      <c r="Q11" s="25" t="n">
+      <c r="R11" s="25" t="n">
         <v>0.9833333333333334</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="12">
       <c r="A12" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="23" t="inlineStr">
         <is>
@@ -1541,51 +1571,54 @@
         <f>IFERROR(SUM(0.5*E12,0.5*F12),0)</f>
       </c>
       <c r="E12" s="26" t="str">
-        <f>IFERROR(AVERAGE(G12,J12,M12,O12),0)</f>
+        <f>IFERROR(AVERAGE(G12,H12,K12,N12,P12),0)</f>
       </c>
       <c r="F12" s="26" t="str">
-        <f>IFERROR(AVERAGE(H12,I12,K12,L12,N12,P12,Q12),0)</f>
+        <f>IFERROR(AVERAGE(I12,J12,L12,M12,O12,Q12,R12),0)</f>
       </c>
       <c r="G12" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" s="25" t="n">
         <v>0.5</v>
       </c>
-      <c r="H12" s="25" t="n">
+      <c r="I12" s="25" t="n">
         <v>0.9818181818181819</v>
       </c>
-      <c r="I12" s="25" t="n">
+      <c r="J12" s="25" t="n">
         <v>0.975</v>
       </c>
-      <c r="J12" s="25" t="n">
+      <c r="K12" s="25" t="n">
         <v>0.0</v>
       </c>
-      <c r="K12" s="25" t="n">
+      <c r="L12" s="25" t="n">
         <v>0.114</v>
       </c>
-      <c r="L12" s="25" t="n">
+      <c r="M12" s="25" t="n">
         <v>0.98125</v>
       </c>
-      <c r="M12" s="25" t="n">
+      <c r="N12" s="25" t="n">
         <v>0.75</v>
       </c>
-      <c r="N12" s="25" t="n">
+      <c r="O12" s="25" t="n">
         <v>0.8849999999999999</v>
       </c>
-      <c r="O12" s="25" t="n">
+      <c r="P12" s="25" t="n">
         <v>0.75</v>
       </c>
-      <c r="P12" s="25" t="n">
+      <c r="Q12" s="25" t="n">
         <v>0.9763157894736842</v>
       </c>
-      <c r="Q12" s="25" t="n">
+      <c r="R12" s="25" t="n">
         <v>0.9833333333333334</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="13">
       <c r="A13" s="18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13" s="23" t="inlineStr">
         <is>
@@ -1596,51 +1629,54 @@
         <f>IFERROR(SUM(0.5*E13,0.5*F13),0)</f>
       </c>
       <c r="E13" s="26" t="str">
-        <f>IFERROR(AVERAGE(G13,J13,M13,O13),0)</f>
+        <f>IFERROR(AVERAGE(G13,H13,K13,N13,P13),0)</f>
       </c>
       <c r="F13" s="26" t="str">
-        <f>IFERROR(AVERAGE(H13,I13,K13,L13,N13,P13,Q13),0)</f>
+        <f>IFERROR(AVERAGE(I13,J13,L13,M13,O13,Q13,R13),0)</f>
       </c>
       <c r="G13" s="25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H13" s="25" t="n">
         <v>0.7</v>
       </c>
-      <c r="H13" s="25" t="n">
+      <c r="I13" s="25" t="n">
         <v>0.9727272727272727</v>
       </c>
-      <c r="I13" s="25" t="n">
+      <c r="J13" s="25" t="n">
         <v>0.9800000000000001</v>
       </c>
-      <c r="J13" s="25" t="n">
+      <c r="K13" s="25" t="n">
         <v>0.6363636363636364</v>
       </c>
-      <c r="K13" s="25" t="n">
+      <c r="L13" s="25" t="n">
         <v>0.9666666666666667</v>
       </c>
-      <c r="L13" s="25" t="n">
+      <c r="M13" s="25" t="n">
         <v>0.98125</v>
       </c>
-      <c r="M13" s="25" t="n">
+      <c r="N13" s="25" t="n">
         <v>0.875</v>
       </c>
-      <c r="N13" s="25" t="n">
+      <c r="O13" s="25" t="n">
         <v>0.9833333333333334</v>
       </c>
-      <c r="O13" s="25" t="n">
+      <c r="P13" s="25" t="n">
         <v>0.8125</v>
       </c>
-      <c r="P13" s="25" t="n">
+      <c r="Q13" s="25" t="n">
         <v>0.9763157894736842</v>
       </c>
-      <c r="Q13" s="25" t="n">
+      <c r="R13" s="25" t="n">
         <v>0.9833333333333334</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="14">
       <c r="A14" s="18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C14" s="23" t="inlineStr">
         <is>
@@ -1651,51 +1687,54 @@
         <f>IFERROR(SUM(0.5*E14,0.5*F14),0)</f>
       </c>
       <c r="E14" s="26" t="str">
-        <f>IFERROR(AVERAGE(G14,J14,M14,O14),0)</f>
+        <f>IFERROR(AVERAGE(G14,H14,K14,N14,P14),0)</f>
       </c>
       <c r="F14" s="26" t="str">
-        <f>IFERROR(AVERAGE(H14,I14,K14,L14,N14,P14,Q14),0)</f>
+        <f>IFERROR(AVERAGE(I14,J14,L14,M14,O14,Q14,R14),0)</f>
       </c>
       <c r="G14" s="25" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="H14" s="25" t="n">
         <v>0.7</v>
       </c>
-      <c r="H14" s="25" t="n">
+      <c r="I14" s="25" t="n">
         <v>0.9454545454545454</v>
       </c>
-      <c r="I14" s="25" t="n">
+      <c r="J14" s="25" t="n">
         <v>0.9800000000000001</v>
       </c>
-      <c r="J14" s="25" t="n">
+      <c r="K14" s="25" t="n">
         <v>0.6363636363636364</v>
       </c>
-      <c r="K14" s="25" t="n">
+      <c r="L14" s="25" t="n">
         <v>0.9666666666666667</v>
       </c>
-      <c r="L14" s="25" t="n">
+      <c r="M14" s="25" t="n">
         <v>0.9625</v>
       </c>
-      <c r="M14" s="25" t="n">
+      <c r="N14" s="25" t="n">
         <v>0.75</v>
       </c>
-      <c r="N14" s="25" t="n">
+      <c r="O14" s="25" t="n">
         <v>0.9708333333333333</v>
       </c>
-      <c r="O14" s="25" t="n">
+      <c r="P14" s="25" t="n">
         <v>0.8125</v>
       </c>
-      <c r="P14" s="25" t="n">
+      <c r="Q14" s="25" t="n">
         <v>0.9842105263157894</v>
       </c>
-      <c r="Q14" s="25" t="n">
+      <c r="R14" s="25" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="15">
       <c r="A15" s="18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C15" s="23" t="inlineStr">
         <is>
@@ -1706,51 +1745,54 @@
         <f>IFERROR(SUM(0.5*E15,0.5*F15),0)</f>
       </c>
       <c r="E15" s="26" t="str">
-        <f>IFERROR(AVERAGE(G15,J15,M15,O15),0)</f>
+        <f>IFERROR(AVERAGE(G15,H15,K15,N15,P15),0)</f>
       </c>
       <c r="F15" s="26" t="str">
-        <f>IFERROR(AVERAGE(H15,I15,K15,L15,N15,P15,Q15),0)</f>
+        <f>IFERROR(AVERAGE(I15,J15,L15,M15,O15,Q15,R15),0)</f>
       </c>
       <c r="G15" s="25" t="n">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="H15" s="25" t="n">
         <v>0.7</v>
       </c>
-      <c r="H15" s="25" t="n">
+      <c r="I15" s="25" t="n">
         <v>0.9727272727272727</v>
       </c>
-      <c r="I15" s="25" t="n">
+      <c r="J15" s="25" t="n">
         <v>0.9949999999999999</v>
       </c>
-      <c r="J15" s="25" t="n">
+      <c r="K15" s="25" t="n">
         <v>0.5454545454545454</v>
       </c>
-      <c r="K15" s="25" t="n">
+      <c r="L15" s="25" t="n">
         <v>0.98</v>
       </c>
-      <c r="L15" s="25" t="n">
+      <c r="M15" s="25" t="n">
         <v>0.9875</v>
       </c>
-      <c r="M15" s="25" t="n">
+      <c r="N15" s="25" t="n">
         <v>0.8125</v>
       </c>
-      <c r="N15" s="25" t="n">
+      <c r="O15" s="25" t="n">
         <v>0.9916666666666667</v>
       </c>
-      <c r="O15" s="25" t="n">
+      <c r="P15" s="25" t="n">
         <v>0.625</v>
       </c>
-      <c r="P15" s="25" t="n">
+      <c r="Q15" s="25" t="n">
         <v>0.9684210526315788</v>
       </c>
-      <c r="Q15" s="25" t="n">
+      <c r="R15" s="25" t="n">
         <v>0.9666666666666667</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="16">
       <c r="A16" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" s="23" t="inlineStr">
         <is>
@@ -1761,10 +1803,10 @@
         <f>IFERROR(SUM(0.5*E16,0.5*F16),0)</f>
       </c>
       <c r="E16" s="26" t="str">
-        <f>IFERROR(AVERAGE(G16,J16,M16,O16),0)</f>
+        <f>IFERROR(AVERAGE(G16,H16,K16,N16,P16),0)</f>
       </c>
       <c r="F16" s="26" t="str">
-        <f>IFERROR(AVERAGE(H16,I16,K16,L16,N16,P16,Q16),0)</f>
+        <f>IFERROR(AVERAGE(I16,J16,L16,M16,O16,Q16,R16),0)</f>
       </c>
       <c r="G16" s="25" t="n">
         <v>0.0</v>
@@ -1799,13 +1841,16 @@
       <c r="Q16" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="R16" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="17">
       <c r="A17" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C17" s="23" t="n">
         <v>20624654</v>
@@ -1814,51 +1859,54 @@
         <f>IFERROR(SUM(0.5*E17,0.5*F17),0)</f>
       </c>
       <c r="E17" s="26" t="str">
-        <f>IFERROR(AVERAGE(G17,J17,M17,O17),0)</f>
+        <f>IFERROR(AVERAGE(G17,H17,K17,N17,P17),0)</f>
       </c>
       <c r="F17" s="26" t="str">
-        <f>IFERROR(AVERAGE(H17,I17,K17,L17,N17,P17,Q17),0)</f>
+        <f>IFERROR(AVERAGE(I17,J17,L17,M17,O17,Q17,R17),0)</f>
       </c>
       <c r="G17" s="25" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="H17" s="25" t="n">
         <v>0.8</v>
       </c>
-      <c r="H17" s="25" t="n">
+      <c r="I17" s="25" t="n">
         <v>0.9727272727272727</v>
       </c>
-      <c r="I17" s="25" t="n">
+      <c r="J17" s="25" t="n">
         <v>0.975</v>
       </c>
-      <c r="J17" s="25" t="n">
+      <c r="K17" s="25" t="n">
         <v>0.45454545454545453</v>
       </c>
-      <c r="K17" s="25" t="n">
+      <c r="L17" s="25" t="n">
         <v>0.98</v>
       </c>
-      <c r="L17" s="25" t="n">
+      <c r="M17" s="25" t="n">
         <v>0.9875</v>
       </c>
-      <c r="M17" s="25" t="n">
+      <c r="N17" s="25" t="n">
         <v>0.875</v>
       </c>
-      <c r="N17" s="25" t="n">
+      <c r="O17" s="25" t="n">
         <v>0.9833333333333334</v>
       </c>
-      <c r="O17" s="25" t="n">
+      <c r="P17" s="25" t="n">
         <v>0.875</v>
       </c>
-      <c r="P17" s="25" t="n">
+      <c r="Q17" s="25" t="n">
         <v>0.9447368421052631</v>
       </c>
-      <c r="Q17" s="25" t="n">
+      <c r="R17" s="25" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="18">
       <c r="A18" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C18" s="23" t="inlineStr">
         <is>
@@ -1869,10 +1917,10 @@
         <f>IFERROR(SUM(0.5*E18,0.5*F18),0)</f>
       </c>
       <c r="E18" s="26" t="str">
-        <f>IFERROR(AVERAGE(G18,J18,M18,O18),0)</f>
+        <f>IFERROR(AVERAGE(G18,H18,K18,N18,P18),0)</f>
       </c>
       <c r="F18" s="26" t="str">
-        <f>IFERROR(AVERAGE(H18,I18,K18,L18,N18,P18,Q18),0)</f>
+        <f>IFERROR(AVERAGE(I18,J18,L18,M18,O18,Q18,R18),0)</f>
       </c>
       <c r="G18" s="25" t="n">
         <v>0.0</v>
@@ -1907,13 +1955,16 @@
       <c r="Q18" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="R18" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="19">
       <c r="A19" s="18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C19" s="23" t="inlineStr">
         <is>
@@ -1924,51 +1975,54 @@
         <f>IFERROR(SUM(0.5*E19,0.5*F19),0)</f>
       </c>
       <c r="E19" s="26" t="str">
-        <f>IFERROR(AVERAGE(G19,J19,M19,O19),0)</f>
+        <f>IFERROR(AVERAGE(G19,H19,K19,N19,P19),0)</f>
       </c>
       <c r="F19" s="26" t="str">
-        <f>IFERROR(AVERAGE(H19,I19,K19,L19,N19,P19,Q19),0)</f>
+        <f>IFERROR(AVERAGE(I19,J19,L19,M19,O19,Q19,R19),0)</f>
       </c>
       <c r="G19" s="25" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="H19" s="25" t="n">
         <v>0.8</v>
       </c>
-      <c r="H19" s="25" t="n">
+      <c r="I19" s="25" t="n">
         <v>0.9818181818181819</v>
       </c>
-      <c r="I19" s="25" t="n">
+      <c r="J19" s="25" t="n">
         <v>0.9800000000000001</v>
       </c>
-      <c r="J19" s="25" t="n">
+      <c r="K19" s="25" t="n">
         <v>0.7272727272727273</v>
       </c>
-      <c r="K19" s="25" t="n">
+      <c r="L19" s="25" t="n">
         <v>0.9866666666666667</v>
       </c>
-      <c r="L19" s="25" t="n">
+      <c r="M19" s="25" t="n">
         <v>0.9625</v>
       </c>
-      <c r="M19" s="25" t="n">
+      <c r="N19" s="25" t="n">
         <v>0.875</v>
       </c>
-      <c r="N19" s="25" t="n">
+      <c r="O19" s="25" t="n">
         <v>1.0</v>
       </c>
-      <c r="O19" s="25" t="n">
+      <c r="P19" s="25" t="n">
         <v>0.875</v>
       </c>
-      <c r="P19" s="25" t="n">
+      <c r="Q19" s="25" t="n">
         <v>0.9842105263157894</v>
       </c>
-      <c r="Q19" s="25" t="n">
+      <c r="R19" s="25" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="20">
       <c r="A20" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C20" s="23" t="inlineStr">
         <is>
@@ -1979,51 +2033,54 @@
         <f>IFERROR(SUM(0.5*E20,0.5*F20),0)</f>
       </c>
       <c r="E20" s="26" t="str">
-        <f>IFERROR(AVERAGE(G20,J20,M20,O20),0)</f>
+        <f>IFERROR(AVERAGE(G20,H20,K20,N20,P20),0)</f>
       </c>
       <c r="F20" s="26" t="str">
-        <f>IFERROR(AVERAGE(H20,I20,K20,L20,N20,P20,Q20),0)</f>
+        <f>IFERROR(AVERAGE(I20,J20,L20,M20,O20,Q20,R20),0)</f>
       </c>
       <c r="G20" s="25" t="n">
         <v>1.0</v>
       </c>
       <c r="H20" s="25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I20" s="25" t="n">
         <v>0.9636363636363636</v>
       </c>
-      <c r="I20" s="25" t="n">
+      <c r="J20" s="25" t="n">
         <v>0.9650000000000001</v>
       </c>
-      <c r="J20" s="25" t="n">
+      <c r="K20" s="25" t="n">
         <v>0.45454545454545453</v>
       </c>
-      <c r="K20" s="25" t="n">
+      <c r="L20" s="25" t="n">
         <v>0.9666666666666667</v>
       </c>
-      <c r="L20" s="25" t="n">
+      <c r="M20" s="25" t="n">
         <v>0.975</v>
       </c>
-      <c r="M20" s="25" t="n">
+      <c r="N20" s="25" t="n">
         <v>0.9375</v>
       </c>
-      <c r="N20" s="25" t="n">
+      <c r="O20" s="25" t="n">
         <v>0.975</v>
       </c>
-      <c r="O20" s="25" t="n">
+      <c r="P20" s="25" t="n">
         <v>0.875</v>
       </c>
-      <c r="P20" s="25" t="n">
+      <c r="Q20" s="25" t="n">
         <v>0.9526315789473685</v>
       </c>
-      <c r="Q20" s="25" t="n">
+      <c r="R20" s="25" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="21">
       <c r="A21" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C21" s="23" t="n">
         <v>20589448</v>
@@ -2032,51 +2089,54 @@
         <f>IFERROR(SUM(0.5*E21,0.5*F21),0)</f>
       </c>
       <c r="E21" s="26" t="str">
-        <f>IFERROR(AVERAGE(G21,J21,M21,O21),0)</f>
+        <f>IFERROR(AVERAGE(G21,H21,K21,N21,P21),0)</f>
       </c>
       <c r="F21" s="26" t="str">
-        <f>IFERROR(AVERAGE(H21,I21,K21,L21,N21,P21,Q21),0)</f>
+        <f>IFERROR(AVERAGE(I21,J21,L21,M21,O21,Q21,R21),0)</f>
       </c>
       <c r="G21" s="25" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="H21" s="25" t="n">
         <v>0.8</v>
       </c>
-      <c r="H21" s="25" t="n">
+      <c r="I21" s="25" t="n">
         <v>0.8918181818181818</v>
       </c>
-      <c r="I21" s="25" t="n">
+      <c r="J21" s="25" t="n">
         <v>0.0</v>
       </c>
-      <c r="J21" s="25" t="n">
+      <c r="K21" s="25" t="n">
         <v>0.36363636363636365</v>
       </c>
-      <c r="K21" s="25" t="n">
+      <c r="L21" s="25" t="n">
         <v>0.9266666666666666</v>
       </c>
-      <c r="L21" s="25" t="n">
+      <c r="M21" s="25" t="n">
         <v>0.855</v>
       </c>
-      <c r="M21" s="25" t="n">
+      <c r="N21" s="25" t="n">
         <v>0.625</v>
       </c>
-      <c r="N21" s="25" t="n">
+      <c r="O21" s="25" t="n">
         <v>0.9874999999999999</v>
       </c>
-      <c r="O21" s="25" t="n">
+      <c r="P21" s="25" t="n">
         <v>0.5625</v>
       </c>
-      <c r="P21" s="25" t="n">
+      <c r="Q21" s="25" t="n">
         <v>0.9428947368421052</v>
       </c>
-      <c r="Q21" s="25" t="n">
+      <c r="R21" s="25" t="n">
         <v>0.9333333333333332</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="22">
       <c r="A22" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C22" s="23" t="inlineStr">
         <is>
@@ -2087,51 +2147,54 @@
         <f>IFERROR(SUM(0.5*E22,0.5*F22),0)</f>
       </c>
       <c r="E22" s="26" t="str">
-        <f>IFERROR(AVERAGE(G22,J22,M22,O22),0)</f>
+        <f>IFERROR(AVERAGE(G22,H22,K22,N22,P22),0)</f>
       </c>
       <c r="F22" s="26" t="str">
-        <f>IFERROR(AVERAGE(H22,I22,K22,L22,N22,P22,Q22),0)</f>
+        <f>IFERROR(AVERAGE(I22,J22,L22,M22,O22,Q22,R22),0)</f>
       </c>
       <c r="G22" s="25" t="n">
-        <v>0.0</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="H22" s="25" t="n">
         <v>0.0</v>
       </c>
       <c r="I22" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J22" s="25" t="n">
         <v>0.99</v>
       </c>
-      <c r="J22" s="25" t="n">
+      <c r="K22" s="25" t="n">
         <v>0.36363636363636365</v>
       </c>
-      <c r="K22" s="25" t="n">
+      <c r="L22" s="25" t="n">
         <v>0.98</v>
       </c>
-      <c r="L22" s="25" t="n">
+      <c r="M22" s="25" t="n">
         <v>0.9875</v>
       </c>
-      <c r="M22" s="25" t="n">
+      <c r="N22" s="25" t="n">
         <v>0.8125</v>
       </c>
-      <c r="N22" s="25" t="n">
+      <c r="O22" s="25" t="n">
         <v>0.9874999999999999</v>
       </c>
-      <c r="O22" s="25" t="n">
+      <c r="P22" s="25" t="n">
         <v>0.875</v>
       </c>
-      <c r="P22" s="25" t="n">
+      <c r="Q22" s="25" t="n">
         <v>0.9763157894736842</v>
       </c>
-      <c r="Q22" s="25" t="n">
+      <c r="R22" s="25" t="n">
         <v>0.9833333333333334</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="23">
       <c r="A23" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C23" s="23" t="n">
         <v>20554069</v>
@@ -2140,51 +2203,54 @@
         <f>IFERROR(SUM(0.5*E23,0.5*F23),0)</f>
       </c>
       <c r="E23" s="26" t="str">
-        <f>IFERROR(AVERAGE(G23,J23,M23,O23),0)</f>
+        <f>IFERROR(AVERAGE(G23,H23,K23,N23,P23),0)</f>
       </c>
       <c r="F23" s="26" t="str">
-        <f>IFERROR(AVERAGE(H23,I23,K23,L23,N23,P23,Q23),0)</f>
+        <f>IFERROR(AVERAGE(I23,J23,L23,M23,O23,Q23,R23),0)</f>
       </c>
       <c r="G23" s="25" t="n">
+        <v>0.7714285714285715</v>
+      </c>
+      <c r="H23" s="25" t="n">
         <v>0.6</v>
       </c>
-      <c r="H23" s="25" t="n">
+      <c r="I23" s="25" t="n">
         <v>0.9727272727272727</v>
       </c>
-      <c r="I23" s="25" t="n">
+      <c r="J23" s="25" t="n">
         <v>0.97</v>
       </c>
-      <c r="J23" s="25" t="n">
+      <c r="K23" s="25" t="n">
         <v>0.5454545454545454</v>
       </c>
-      <c r="K23" s="25" t="n">
+      <c r="L23" s="25" t="n">
         <v>0.98</v>
       </c>
-      <c r="L23" s="25" t="n">
+      <c r="M23" s="25" t="n">
         <v>0.883125</v>
       </c>
-      <c r="M23" s="25" t="n">
+      <c r="N23" s="25" t="n">
         <v>0.875</v>
       </c>
-      <c r="N23" s="25" t="n">
+      <c r="O23" s="25" t="n">
         <v>0.9916666666666667</v>
       </c>
-      <c r="O23" s="25" t="n">
+      <c r="P23" s="25" t="n">
         <v>0.75</v>
       </c>
-      <c r="P23" s="25" t="n">
+      <c r="Q23" s="25" t="n">
         <v>0.9526315789473685</v>
       </c>
-      <c r="Q23" s="25" t="n">
+      <c r="R23" s="25" t="n">
         <v>0.9833333333333334</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="24">
       <c r="A24" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C24" s="23" t="inlineStr">
         <is>
@@ -2195,51 +2261,54 @@
         <f>IFERROR(SUM(0.5*E24,0.5*F24),0)</f>
       </c>
       <c r="E24" s="26" t="str">
-        <f>IFERROR(AVERAGE(G24,J24,M24,O24),0)</f>
+        <f>IFERROR(AVERAGE(G24,H24,K24,N24,P24),0)</f>
       </c>
       <c r="F24" s="26" t="str">
-        <f>IFERROR(AVERAGE(H24,I24,K24,L24,N24,P24,Q24),0)</f>
+        <f>IFERROR(AVERAGE(I24,J24,L24,M24,O24,Q24,R24),0)</f>
       </c>
       <c r="G24" s="25" t="n">
         <v>0.9</v>
       </c>
       <c r="H24" s="25" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="I24" s="25" t="n">
         <v>0.9636363636363636</v>
       </c>
-      <c r="I24" s="25" t="n">
+      <c r="J24" s="25" t="n">
         <v>0.95</v>
       </c>
-      <c r="J24" s="25" t="n">
+      <c r="K24" s="25" t="n">
         <v>0.5454545454545454</v>
       </c>
-      <c r="K24" s="25" t="n">
+      <c r="L24" s="25" t="n">
         <v>0.94</v>
       </c>
-      <c r="L24" s="25" t="n">
+      <c r="M24" s="25" t="n">
         <v>0.9375</v>
       </c>
-      <c r="M24" s="25" t="n">
+      <c r="N24" s="25" t="n">
         <v>0.8125</v>
       </c>
-      <c r="N24" s="25" t="n">
+      <c r="O24" s="25" t="n">
         <v>0.9583333333333334</v>
       </c>
-      <c r="O24" s="25" t="n">
+      <c r="P24" s="25" t="n">
         <v>0.8125</v>
       </c>
-      <c r="P24" s="25" t="n">
+      <c r="Q24" s="25" t="n">
         <v>0.9289473684210525</v>
       </c>
-      <c r="Q24" s="25" t="n">
+      <c r="R24" s="25" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="25">
       <c r="A25" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C25" s="23" t="inlineStr">
         <is>
@@ -2250,51 +2319,54 @@
         <f>IFERROR(SUM(0.5*E25,0.5*F25),0)</f>
       </c>
       <c r="E25" s="26" t="str">
-        <f>IFERROR(AVERAGE(G25,J25,M25,O25),0)</f>
+        <f>IFERROR(AVERAGE(G25,H25,K25,N25,P25),0)</f>
       </c>
       <c r="F25" s="26" t="str">
-        <f>IFERROR(AVERAGE(H25,I25,K25,L25,N25,P25,Q25),0)</f>
+        <f>IFERROR(AVERAGE(I25,J25,L25,M25,O25,Q25,R25),0)</f>
       </c>
       <c r="G25" s="25" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="H25" s="25" t="n">
         <v>0.7</v>
       </c>
-      <c r="H25" s="25" t="n">
+      <c r="I25" s="25" t="n">
         <v>0.859090909090909</v>
       </c>
-      <c r="I25" s="25" t="n">
+      <c r="J25" s="25" t="n">
         <v>0.99</v>
       </c>
-      <c r="J25" s="25" t="n">
+      <c r="K25" s="25" t="n">
         <v>0.36363636363636365</v>
       </c>
-      <c r="K25" s="25" t="n">
+      <c r="L25" s="25" t="n">
         <v>0.9673333333333333</v>
       </c>
-      <c r="L25" s="25" t="n">
+      <c r="M25" s="25" t="n">
         <v>0.883125</v>
       </c>
-      <c r="M25" s="25" t="n">
+      <c r="N25" s="25" t="n">
         <v>0.6875</v>
       </c>
-      <c r="N25" s="25" t="n">
+      <c r="O25" s="25" t="n">
         <v>0.9791666666666666</v>
       </c>
-      <c r="O25" s="25" t="n">
+      <c r="P25" s="25" t="n">
         <v>0.9375</v>
       </c>
-      <c r="P25" s="25" t="n">
+      <c r="Q25" s="25" t="n">
         <v>0.935</v>
       </c>
-      <c r="Q25" s="25" t="n">
+      <c r="R25" s="25" t="n">
         <v>0.8849999999999999</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="26">
       <c r="A26" s="18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C26" s="23" t="n">
         <v>20610517</v>
@@ -2303,10 +2375,10 @@
         <f>IFERROR(SUM(0.5*E26,0.5*F26),0)</f>
       </c>
       <c r="E26" s="26" t="str">
-        <f>IFERROR(AVERAGE(G26,J26,M26,O26),0)</f>
+        <f>IFERROR(AVERAGE(G26,H26,K26,N26,P26),0)</f>
       </c>
       <c r="F26" s="26" t="str">
-        <f>IFERROR(AVERAGE(H26,I26,K26,L26,N26,P26,Q26),0)</f>
+        <f>IFERROR(AVERAGE(I26,J26,L26,M26,O26,Q26,R26),0)</f>
       </c>
       <c r="G26" s="25" t="n">
         <v>1.0</v>
@@ -2315,39 +2387,42 @@
         <v>1.0</v>
       </c>
       <c r="I26" s="25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J26" s="25" t="n">
         <v>0.9949999999999999</v>
       </c>
-      <c r="J26" s="25" t="n">
+      <c r="K26" s="25" t="n">
         <v>0.5454545454545454</v>
       </c>
-      <c r="K26" s="25" t="n">
+      <c r="L26" s="25" t="n">
         <v>0.9933333333333334</v>
       </c>
-      <c r="L26" s="25" t="n">
+      <c r="M26" s="25" t="n">
         <v>0.9875</v>
       </c>
-      <c r="M26" s="25" t="n">
+      <c r="N26" s="25" t="n">
         <v>0.9375</v>
       </c>
-      <c r="N26" s="25" t="n">
+      <c r="O26" s="25" t="n">
         <v>0.975</v>
       </c>
-      <c r="O26" s="25" t="n">
+      <c r="P26" s="25" t="n">
         <v>0.75</v>
       </c>
-      <c r="P26" s="25" t="n">
+      <c r="Q26" s="25" t="n">
         <v>0.9921052631578948</v>
       </c>
-      <c r="Q26" s="25" t="n">
+      <c r="R26" s="25" t="n">
         <v>0.87</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="27">
       <c r="A27" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C27" s="23" t="inlineStr">
         <is>
@@ -2358,51 +2433,54 @@
         <f>IFERROR(SUM(0.5*E27,0.5*F27),0)</f>
       </c>
       <c r="E27" s="26" t="str">
-        <f>IFERROR(AVERAGE(G27,J27,M27,O27),0)</f>
+        <f>IFERROR(AVERAGE(G27,H27,K27,N27,P27),0)</f>
       </c>
       <c r="F27" s="26" t="str">
-        <f>IFERROR(AVERAGE(H27,I27,K27,L27,N27,P27,Q27),0)</f>
+        <f>IFERROR(AVERAGE(I27,J27,L27,M27,O27,Q27,R27),0)</f>
       </c>
       <c r="G27" s="25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H27" s="25" t="n">
         <v>0.7</v>
       </c>
-      <c r="H27" s="25" t="n">
+      <c r="I27" s="25" t="n">
         <v>0.9636363636363636</v>
       </c>
-      <c r="I27" s="25" t="n">
+      <c r="J27" s="25" t="n">
         <v>0.985</v>
       </c>
-      <c r="J27" s="25" t="n">
+      <c r="K27" s="25" t="n">
         <v>0.36363636363636365</v>
       </c>
-      <c r="K27" s="25" t="n">
+      <c r="L27" s="25" t="n">
         <v>0.9666666666666667</v>
       </c>
-      <c r="L27" s="25" t="n">
+      <c r="M27" s="25" t="n">
         <v>0.9875</v>
       </c>
-      <c r="M27" s="25" t="n">
+      <c r="N27" s="25" t="n">
         <v>0.9375</v>
       </c>
-      <c r="N27" s="25" t="n">
+      <c r="O27" s="25" t="n">
         <v>0.9791666666666666</v>
       </c>
-      <c r="O27" s="25" t="n">
+      <c r="P27" s="25" t="n">
         <v>0.75</v>
       </c>
-      <c r="P27" s="25" t="n">
+      <c r="Q27" s="25" t="n">
         <v>0.9763157894736842</v>
       </c>
-      <c r="Q27" s="25" t="n">
+      <c r="R27" s="25" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="28">
       <c r="A28" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C28" s="23" t="inlineStr">
         <is>
@@ -2413,13 +2491,13 @@
         <f>IFERROR(SUM(0.5*E28,0.5*F28),0)</f>
       </c>
       <c r="E28" s="26" t="str">
-        <f>IFERROR(AVERAGE(G28,J28,M28,O28),0)</f>
+        <f>IFERROR(AVERAGE(G28,H28,K28,N28,P28),0)</f>
       </c>
       <c r="F28" s="26" t="str">
-        <f>IFERROR(AVERAGE(H28,I28,K28,L28,N28,P28,Q28),0)</f>
+        <f>IFERROR(AVERAGE(I28,J28,L28,M28,O28,Q28,R28),0)</f>
       </c>
       <c r="G28" s="25" t="n">
-        <v>0.0</v>
+        <v>0.9</v>
       </c>
       <c r="H28" s="25" t="n">
         <v>0.0</v>
@@ -2428,36 +2506,39 @@
         <v>0.0</v>
       </c>
       <c r="J28" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K28" s="25" t="n">
         <v>0.45454545454545453</v>
       </c>
-      <c r="K28" s="25" t="n">
+      <c r="L28" s="25" t="n">
         <v>0.9733333333333333</v>
       </c>
-      <c r="L28" s="25" t="n">
+      <c r="M28" s="25" t="n">
         <v>0.95625</v>
       </c>
-      <c r="M28" s="25" t="n">
+      <c r="N28" s="25" t="n">
         <v>0.8125</v>
       </c>
-      <c r="N28" s="25" t="n">
+      <c r="O28" s="25" t="n">
         <v>0.87</v>
       </c>
-      <c r="O28" s="25" t="n">
+      <c r="P28" s="25" t="n">
         <v>1.0</v>
       </c>
-      <c r="P28" s="25" t="n">
+      <c r="Q28" s="25" t="n">
         <v>0.9210526315789473</v>
       </c>
-      <c r="Q28" s="25" t="n">
+      <c r="R28" s="25" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="29">
       <c r="A29" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C29" s="23" t="inlineStr">
         <is>
@@ -2468,48 +2549,51 @@
         <f>IFERROR(SUM(0.5*E29,0.5*F29),0)</f>
       </c>
       <c r="E29" s="26" t="str">
-        <f>IFERROR(AVERAGE(G29,J29,M29,O29),0)</f>
+        <f>IFERROR(AVERAGE(G29,H29,K29,N29,P29),0)</f>
       </c>
       <c r="F29" s="26" t="str">
-        <f>IFERROR(AVERAGE(H29,I29,K29,L29,N29,P29,Q29),0)</f>
+        <f>IFERROR(AVERAGE(I29,J29,L29,M29,O29,Q29,R29),0)</f>
       </c>
       <c r="G29" s="25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H29" s="25" t="n">
         <v>0.9</v>
       </c>
-      <c r="H29" s="25" t="n">
+      <c r="I29" s="25" t="n">
         <v>0.9454545454545454</v>
       </c>
-      <c r="I29" s="25" t="n">
+      <c r="J29" s="25" t="n">
         <v>0.975</v>
       </c>
-      <c r="J29" s="25" t="n">
+      <c r="K29" s="25" t="n">
         <v>0.6363636363636364</v>
       </c>
-      <c r="K29" s="25" t="n">
+      <c r="L29" s="25" t="n">
         <v>0.9600000000000001</v>
       </c>
-      <c r="L29" s="25" t="n">
+      <c r="M29" s="25" t="n">
         <v>0.9875</v>
       </c>
-      <c r="M29" s="25" t="n">
+      <c r="N29" s="25" t="n">
         <v>0.875</v>
       </c>
-      <c r="N29" s="25" t="n">
+      <c r="O29" s="25" t="n">
         <v>0.8849999999999999</v>
       </c>
-      <c r="O29" s="25" t="n">
+      <c r="P29" s="25" t="n">
         <v>0.875</v>
       </c>
-      <c r="P29" s="25" t="n">
+      <c r="Q29" s="25" t="n">
         <v>0.9842105263157894</v>
       </c>
-      <c r="Q29" s="25" t="n">
+      <c r="R29" s="25" t="n">
         <v>0.9833333333333334</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="30">
       <c r="A30" s="28" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B30" s="29" t="inlineStr">
         <is>
@@ -2563,10 +2647,13 @@
       <c r="Q30" s="39" t="str">
         <f>IFERROR(AVERAGE(Q11:Q29),"")</f>
       </c>
+      <c r="R30" s="39" t="str">
+        <f>IFERROR(AVERAGE(R11:R29),"")</f>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="31">
       <c r="A31" s="47" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B31" s="48" t="inlineStr">
         <is>
@@ -2620,10 +2707,13 @@
       <c r="Q31" s="38" t="str">
         <f>IFERROR(MIN(Q11:Q29),"")</f>
       </c>
+      <c r="R31" s="38" t="str">
+        <f>IFERROR(MIN(R11:R29),"")</f>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="32">
       <c r="A32" s="47" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B32" s="48" t="inlineStr">
         <is>
@@ -2676,6 +2766,9 @@
       </c>
       <c r="Q32" s="38" t="str">
         <f>IFERROR(MAX(Q11:Q29),"")</f>
+      </c>
+      <c r="R32" s="38" t="str">
+        <f>IFERROR(MAX(R11:R29),"")</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="33"/>
@@ -2685,7 +2778,7 @@
     <row customHeight="1" ht="15" r="37"/>
     <row customHeight="1" ht="15" r="38">
       <c r="A38" s="50" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B38" s="50" t="inlineStr">
         <is>
@@ -2763,6 +2856,11 @@
         </is>
       </c>
       <c r="Q38" s="50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R38" s="50" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2850,6 +2948,11 @@
         </is>
       </c>
       <c r="Q39" s="51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="R39" s="51" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -2860,12 +2963,12 @@
     <row customHeight="1" ht="15" r="42"/>
     <row customHeight="1" ht="15" r="43">
       <c r="A43" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <mergeCells count="18">
+  <mergeCells count="19">
     <mergeCell ref="D7:F8"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
@@ -2881,6 +2984,7 @@
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="P9:P10"/>
     <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R9:R10"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A32:C32"/>
@@ -2897,7 +3001,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0">
       <pane topLeftCell="D11" state="frozen" activePane="bottomRight" ySplit="10" xSplit="3"/>
@@ -2930,6 +3034,8 @@
     <col min="23" max="23" bestFit="1" customWidth="1" width="16"/>
     <col min="24" max="24" bestFit="1" customWidth="1" width="16"/>
     <col min="25" max="25" bestFit="1" customWidth="1" width="16"/>
+    <col min="26" max="26" bestFit="1" customWidth="1" width="16"/>
+    <col min="27" max="27" bestFit="1" customWidth="1" width="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3015,6 +3121,9 @@
       <c r="N7" s="10" t="s">
         <v>15</v>
       </c>
+      <c r="O7" s="10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="8">
       <c r="A8" s="0" t="inlineStr">
@@ -3033,37 +3142,40 @@
         </is>
       </c>
       <c r="D8" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="9">
@@ -3083,48 +3195,51 @@
         </is>
       </c>
       <c r="D9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="O9" s="15" t="s">
+        <v>30</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="10">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" s="15" t="inlineStr">
         <is>
@@ -3181,7 +3296,7 @@
           <t/>
         </is>
       </c>
-      <c r="O10" s="0" t="inlineStr">
+      <c r="O10" s="15" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -3232,6 +3347,16 @@
         </is>
       </c>
       <c r="Y10" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z10" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA10" s="0" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -3239,10 +3364,10 @@
     </row>
     <row customHeight="1" ht="15" r="11">
       <c r="A11" s="18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="23" t="inlineStr">
         <is>
@@ -3250,45 +3375,48 @@
         </is>
       </c>
       <c r="D11" s="20" t="str">
+        <f>ROUND(7.0, 2)</f>
+      </c>
+      <c r="E11" s="20" t="str">
         <f>ROUND(10.0, 2)</f>
       </c>
-      <c r="E11" s="20" t="str">
+      <c r="F11" s="20" t="str">
         <f>ROUND(10.4, 2)</f>
       </c>
-      <c r="F11" s="20" t="str">
+      <c r="G11" s="20" t="str">
         <f>ROUND(19.4, 2)</f>
       </c>
-      <c r="G11" s="20" t="str">
+      <c r="H11" s="20" t="str">
         <f>ROUND(8.0, 2)</f>
       </c>
-      <c r="H11" s="20" t="str">
+      <c r="I11" s="20" t="str">
         <f>ROUND(14.4, 2)</f>
       </c>
-      <c r="I11" s="20" t="str">
+      <c r="J11" s="20" t="str">
         <f>ROUND(15.6, 2)</f>
       </c>
-      <c r="J11" s="20" t="str">
+      <c r="K11" s="20" t="str">
         <f>ROUND(11.0, 2)</f>
       </c>
-      <c r="K11" s="20" t="str">
+      <c r="L11" s="20" t="str">
         <f>ROUND(23.7, 2)</f>
       </c>
-      <c r="L11" s="20" t="str">
+      <c r="M11" s="20" t="str">
         <f>ROUND(13.0, 2)</f>
       </c>
-      <c r="M11" s="20" t="str">
+      <c r="N11" s="20" t="str">
         <f>ROUND(18.4, 2)</f>
       </c>
-      <c r="N11" s="20" t="str">
+      <c r="O11" s="20" t="str">
         <f>ROUND(5.9, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="12">
       <c r="A12" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="23" t="inlineStr">
         <is>
@@ -3296,45 +3424,48 @@
         </is>
       </c>
       <c r="D12" s="20" t="str">
+        <f>ROUND(0.0, 2)</f>
+      </c>
+      <c r="E12" s="20" t="str">
         <f>ROUND(5.0, 2)</f>
       </c>
-      <c r="E12" s="20" t="str">
+      <c r="F12" s="20" t="str">
         <f>ROUND(10.8, 2)</f>
       </c>
-      <c r="F12" s="20" t="str">
+      <c r="G12" s="20" t="str">
         <f>ROUND(19.5, 2)</f>
       </c>
-      <c r="G12" s="20" t="str">
+      <c r="H12" s="20" t="str">
         <f>ROUND(0.0, 2)</f>
       </c>
-      <c r="H12" s="20" t="str">
+      <c r="I12" s="20" t="str">
         <f>ROUND(1.71, 2)</f>
       </c>
-      <c r="I12" s="20" t="str">
+      <c r="J12" s="20" t="str">
         <f>ROUND(15.7, 2)</f>
       </c>
-      <c r="J12" s="20" t="str">
+      <c r="K12" s="20" t="str">
         <f>ROUND(12.0, 2)</f>
       </c>
-      <c r="K12" s="20" t="str">
+      <c r="L12" s="20" t="str">
         <f>ROUND(21.24, 2)</f>
       </c>
-      <c r="L12" s="20" t="str">
+      <c r="M12" s="20" t="str">
         <f>ROUND(12.0, 2)</f>
       </c>
-      <c r="M12" s="20" t="str">
+      <c r="N12" s="20" t="str">
         <f>ROUND(18.55, 2)</f>
       </c>
-      <c r="N12" s="20" t="str">
+      <c r="O12" s="20" t="str">
         <f>ROUND(5.9, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="13">
       <c r="A13" s="18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13" s="23" t="inlineStr">
         <is>
@@ -3345,42 +3476,45 @@
         <f>ROUND(7.0, 2)</f>
       </c>
       <c r="E13" s="20" t="str">
+        <f>ROUND(7.0, 2)</f>
+      </c>
+      <c r="F13" s="20" t="str">
         <f>ROUND(10.7, 2)</f>
       </c>
-      <c r="F13" s="20" t="str">
+      <c r="G13" s="20" t="str">
         <f>ROUND(19.6, 2)</f>
       </c>
-      <c r="G13" s="20" t="str">
+      <c r="H13" s="20" t="str">
         <f>ROUND(7.0, 2)</f>
       </c>
-      <c r="H13" s="20" t="str">
+      <c r="I13" s="20" t="str">
         <f>ROUND(14.5, 2)</f>
       </c>
-      <c r="I13" s="20" t="str">
+      <c r="J13" s="20" t="str">
         <f>ROUND(15.7, 2)</f>
       </c>
-      <c r="J13" s="20" t="str">
+      <c r="K13" s="20" t="str">
         <f>ROUND(14.0, 2)</f>
       </c>
-      <c r="K13" s="20" t="str">
+      <c r="L13" s="20" t="str">
         <f>ROUND(23.6, 2)</f>
       </c>
-      <c r="L13" s="20" t="str">
+      <c r="M13" s="20" t="str">
         <f>ROUND(13.0, 2)</f>
       </c>
-      <c r="M13" s="20" t="str">
+      <c r="N13" s="20" t="str">
         <f>ROUND(18.55, 2)</f>
       </c>
-      <c r="N13" s="20" t="str">
+      <c r="O13" s="20" t="str">
         <f>ROUND(5.9, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="14">
       <c r="A14" s="18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C14" s="23" t="inlineStr">
         <is>
@@ -3388,45 +3522,48 @@
         </is>
       </c>
       <c r="D14" s="20" t="str">
+        <f>ROUND(6.0, 2)</f>
+      </c>
+      <c r="E14" s="20" t="str">
         <f>ROUND(7.0, 2)</f>
       </c>
-      <c r="E14" s="20" t="str">
+      <c r="F14" s="20" t="str">
         <f>ROUND(10.4, 2)</f>
       </c>
-      <c r="F14" s="20" t="str">
+      <c r="G14" s="20" t="str">
         <f>ROUND(19.6, 2)</f>
       </c>
-      <c r="G14" s="20" t="str">
+      <c r="H14" s="20" t="str">
         <f>ROUND(7.0, 2)</f>
       </c>
-      <c r="H14" s="20" t="str">
+      <c r="I14" s="20" t="str">
         <f>ROUND(14.5, 2)</f>
       </c>
-      <c r="I14" s="20" t="str">
+      <c r="J14" s="20" t="str">
         <f>ROUND(15.4, 2)</f>
       </c>
-      <c r="J14" s="20" t="str">
+      <c r="K14" s="20" t="str">
         <f>ROUND(12.0, 2)</f>
       </c>
-      <c r="K14" s="20" t="str">
+      <c r="L14" s="20" t="str">
         <f>ROUND(23.3, 2)</f>
       </c>
-      <c r="L14" s="20" t="str">
+      <c r="M14" s="20" t="str">
         <f>ROUND(13.0, 2)</f>
       </c>
-      <c r="M14" s="20" t="str">
+      <c r="N14" s="20" t="str">
         <f>ROUND(18.7, 2)</f>
       </c>
-      <c r="N14" s="20" t="str">
+      <c r="O14" s="20" t="str">
         <f>ROUND(0.0, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="15">
       <c r="A15" s="18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C15" s="23" t="inlineStr">
         <is>
@@ -3434,45 +3571,48 @@
         </is>
       </c>
       <c r="D15" s="20" t="str">
+        <f>ROUND(4.0, 2)</f>
+      </c>
+      <c r="E15" s="20" t="str">
         <f>ROUND(7.0, 2)</f>
       </c>
-      <c r="E15" s="20" t="str">
+      <c r="F15" s="20" t="str">
         <f>ROUND(10.7, 2)</f>
       </c>
-      <c r="F15" s="20" t="str">
+      <c r="G15" s="20" t="str">
         <f>ROUND(19.9, 2)</f>
       </c>
-      <c r="G15" s="20" t="str">
+      <c r="H15" s="20" t="str">
         <f>ROUND(6.0, 2)</f>
       </c>
-      <c r="H15" s="20" t="str">
+      <c r="I15" s="20" t="str">
         <f>ROUND(14.7, 2)</f>
       </c>
-      <c r="I15" s="20" t="str">
+      <c r="J15" s="20" t="str">
         <f>ROUND(15.8, 2)</f>
       </c>
-      <c r="J15" s="20" t="str">
+      <c r="K15" s="20" t="str">
         <f>ROUND(13.0, 2)</f>
       </c>
-      <c r="K15" s="20" t="str">
+      <c r="L15" s="20" t="str">
         <f>ROUND(23.8, 2)</f>
       </c>
-      <c r="L15" s="20" t="str">
+      <c r="M15" s="20" t="str">
         <f>ROUND(10.0, 2)</f>
       </c>
-      <c r="M15" s="20" t="str">
+      <c r="N15" s="20" t="str">
         <f>ROUND(18.4, 2)</f>
       </c>
-      <c r="N15" s="20" t="str">
+      <c r="O15" s="20" t="str">
         <f>ROUND(5.8, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="16">
       <c r="A16" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" s="23" t="inlineStr">
         <is>
@@ -3512,57 +3652,63 @@
       <c r="N16" s="20" t="str">
         <f>ROUND(0.0, 2)</f>
       </c>
+      <c r="O16" s="20" t="str">
+        <f>ROUND(0.0, 2)</f>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="17">
       <c r="A17" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C17" s="23" t="n">
         <v>20624654</v>
       </c>
       <c r="D17" s="20" t="str">
+        <f>ROUND(6.0, 2)</f>
+      </c>
+      <c r="E17" s="20" t="str">
         <f>ROUND(8.0, 2)</f>
       </c>
-      <c r="E17" s="20" t="str">
+      <c r="F17" s="20" t="str">
         <f>ROUND(10.7, 2)</f>
       </c>
-      <c r="F17" s="20" t="str">
+      <c r="G17" s="20" t="str">
         <f>ROUND(19.5, 2)</f>
       </c>
-      <c r="G17" s="20" t="str">
+      <c r="H17" s="20" t="str">
         <f>ROUND(5.0, 2)</f>
       </c>
-      <c r="H17" s="20" t="str">
+      <c r="I17" s="20" t="str">
         <f>ROUND(14.7, 2)</f>
       </c>
-      <c r="I17" s="20" t="str">
+      <c r="J17" s="20" t="str">
         <f>ROUND(15.8, 2)</f>
       </c>
-      <c r="J17" s="20" t="str">
+      <c r="K17" s="20" t="str">
         <f>ROUND(14.0, 2)</f>
       </c>
-      <c r="K17" s="20" t="str">
+      <c r="L17" s="20" t="str">
         <f>ROUND(23.6, 2)</f>
       </c>
-      <c r="L17" s="20" t="str">
+      <c r="M17" s="20" t="str">
         <f>ROUND(14.0, 2)</f>
       </c>
-      <c r="M17" s="20" t="str">
+      <c r="N17" s="20" t="str">
         <f>ROUND(17.95, 2)</f>
       </c>
-      <c r="N17" s="20" t="str">
+      <c r="O17" s="20" t="str">
         <f>ROUND(6.0, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="18">
       <c r="A18" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C18" s="23" t="inlineStr">
         <is>
@@ -3602,13 +3748,16 @@
       <c r="N18" s="20" t="str">
         <f>ROUND(0.0, 2)</f>
       </c>
+      <c r="O18" s="20" t="str">
+        <f>ROUND(0.0, 2)</f>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="19">
       <c r="A19" s="18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C19" s="23" t="inlineStr">
         <is>
@@ -3616,45 +3765,48 @@
         </is>
       </c>
       <c r="D19" s="20" t="str">
+        <f>ROUND(6.0, 2)</f>
+      </c>
+      <c r="E19" s="20" t="str">
         <f>ROUND(8.0, 2)</f>
       </c>
-      <c r="E19" s="20" t="str">
+      <c r="F19" s="20" t="str">
         <f>ROUND(10.8, 2)</f>
       </c>
-      <c r="F19" s="20" t="str">
+      <c r="G19" s="20" t="str">
         <f>ROUND(19.6, 2)</f>
       </c>
-      <c r="G19" s="20" t="str">
+      <c r="H19" s="20" t="str">
         <f>ROUND(8.0, 2)</f>
       </c>
-      <c r="H19" s="20" t="str">
+      <c r="I19" s="20" t="str">
         <f>ROUND(14.8, 2)</f>
       </c>
-      <c r="I19" s="20" t="str">
+      <c r="J19" s="20" t="str">
         <f>ROUND(15.4, 2)</f>
       </c>
-      <c r="J19" s="20" t="str">
+      <c r="K19" s="20" t="str">
         <f>ROUND(14.0, 2)</f>
       </c>
-      <c r="K19" s="20" t="str">
+      <c r="L19" s="20" t="str">
         <f>ROUND(24.0, 2)</f>
       </c>
-      <c r="L19" s="20" t="str">
+      <c r="M19" s="20" t="str">
         <f>ROUND(14.0, 2)</f>
       </c>
-      <c r="M19" s="20" t="str">
+      <c r="N19" s="20" t="str">
         <f>ROUND(18.7, 2)</f>
       </c>
-      <c r="N19" s="20" t="str">
+      <c r="O19" s="20" t="str">
         <f>ROUND(6.0, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="20">
       <c r="A20" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C20" s="23" t="inlineStr">
         <is>
@@ -3662,89 +3814,95 @@
         </is>
       </c>
       <c r="D20" s="20" t="str">
+        <f>ROUND(7.0, 2)</f>
+      </c>
+      <c r="E20" s="20" t="str">
         <f>ROUND(10.0, 2)</f>
       </c>
-      <c r="E20" s="20" t="str">
+      <c r="F20" s="20" t="str">
         <f>ROUND(10.6, 2)</f>
       </c>
-      <c r="F20" s="20" t="str">
+      <c r="G20" s="20" t="str">
         <f>ROUND(19.3, 2)</f>
       </c>
-      <c r="G20" s="20" t="str">
+      <c r="H20" s="20" t="str">
         <f>ROUND(5.0, 2)</f>
       </c>
-      <c r="H20" s="20" t="str">
+      <c r="I20" s="20" t="str">
         <f>ROUND(14.5, 2)</f>
       </c>
-      <c r="I20" s="20" t="str">
+      <c r="J20" s="20" t="str">
         <f>ROUND(15.6, 2)</f>
       </c>
-      <c r="J20" s="20" t="str">
+      <c r="K20" s="20" t="str">
         <f>ROUND(15.0, 2)</f>
       </c>
-      <c r="K20" s="20" t="str">
+      <c r="L20" s="20" t="str">
         <f>ROUND(23.4, 2)</f>
       </c>
-      <c r="L20" s="20" t="str">
+      <c r="M20" s="20" t="str">
         <f>ROUND(14.0, 2)</f>
       </c>
-      <c r="M20" s="20" t="str">
+      <c r="N20" s="20" t="str">
         <f>ROUND(18.1, 2)</f>
       </c>
-      <c r="N20" s="20" t="str">
+      <c r="O20" s="20" t="str">
         <f>ROUND(6.0, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="21">
       <c r="A21" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C21" s="23" t="n">
         <v>20589448</v>
       </c>
       <c r="D21" s="20" t="str">
+        <f>ROUND(6.0, 2)</f>
+      </c>
+      <c r="E21" s="20" t="str">
         <f>ROUND(8.0, 2)</f>
       </c>
-      <c r="E21" s="20" t="str">
+      <c r="F21" s="20" t="str">
         <f>ROUND(9.81, 2)</f>
       </c>
-      <c r="F21" s="20" t="str">
+      <c r="G21" s="20" t="str">
         <f>ROUND(0.0, 2)</f>
       </c>
-      <c r="G21" s="20" t="str">
+      <c r="H21" s="20" t="str">
         <f>ROUND(4.0, 2)</f>
       </c>
-      <c r="H21" s="20" t="str">
+      <c r="I21" s="20" t="str">
         <f>ROUND(13.9, 2)</f>
       </c>
-      <c r="I21" s="20" t="str">
+      <c r="J21" s="20" t="str">
         <f>ROUND(13.68, 2)</f>
       </c>
-      <c r="J21" s="20" t="str">
+      <c r="K21" s="20" t="str">
         <f>ROUND(10.0, 2)</f>
       </c>
-      <c r="K21" s="20" t="str">
+      <c r="L21" s="20" t="str">
         <f>ROUND(23.7, 2)</f>
       </c>
-      <c r="L21" s="20" t="str">
+      <c r="M21" s="20" t="str">
         <f>ROUND(9.0, 2)</f>
       </c>
-      <c r="M21" s="20" t="str">
+      <c r="N21" s="20" t="str">
         <f>ROUND(17.915, 2)</f>
       </c>
-      <c r="N21" s="20" t="str">
+      <c r="O21" s="20" t="str">
         <f>ROUND(5.6, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="22">
       <c r="A22" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C22" s="23" t="inlineStr">
         <is>
@@ -3752,89 +3910,95 @@
         </is>
       </c>
       <c r="D22" s="20" t="str">
-        <f>ROUND(0.0, 2)</f>
+        <f>ROUND(6.0, 2)</f>
       </c>
       <c r="E22" s="20" t="str">
         <f>ROUND(0.0, 2)</f>
       </c>
       <c r="F22" s="20" t="str">
+        <f>ROUND(0.0, 2)</f>
+      </c>
+      <c r="G22" s="20" t="str">
         <f>ROUND(19.8, 2)</f>
       </c>
-      <c r="G22" s="20" t="str">
+      <c r="H22" s="20" t="str">
         <f>ROUND(4.0, 2)</f>
       </c>
-      <c r="H22" s="20" t="str">
+      <c r="I22" s="20" t="str">
         <f>ROUND(14.7, 2)</f>
       </c>
-      <c r="I22" s="20" t="str">
+      <c r="J22" s="20" t="str">
         <f>ROUND(15.8, 2)</f>
       </c>
-      <c r="J22" s="20" t="str">
+      <c r="K22" s="20" t="str">
         <f>ROUND(13.0, 2)</f>
       </c>
-      <c r="K22" s="20" t="str">
+      <c r="L22" s="20" t="str">
         <f>ROUND(23.7, 2)</f>
       </c>
-      <c r="L22" s="20" t="str">
+      <c r="M22" s="20" t="str">
         <f>ROUND(14.0, 2)</f>
       </c>
-      <c r="M22" s="20" t="str">
+      <c r="N22" s="20" t="str">
         <f>ROUND(18.55, 2)</f>
       </c>
-      <c r="N22" s="20" t="str">
+      <c r="O22" s="20" t="str">
         <f>ROUND(5.9, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="23">
       <c r="A23" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C23" s="23" t="n">
         <v>20554069</v>
       </c>
       <c r="D23" s="20" t="str">
+        <f>ROUND(5.4, 2)</f>
+      </c>
+      <c r="E23" s="20" t="str">
         <f>ROUND(6.0, 2)</f>
       </c>
-      <c r="E23" s="20" t="str">
+      <c r="F23" s="20" t="str">
         <f>ROUND(10.7, 2)</f>
       </c>
-      <c r="F23" s="20" t="str">
+      <c r="G23" s="20" t="str">
         <f>ROUND(19.4, 2)</f>
       </c>
-      <c r="G23" s="20" t="str">
+      <c r="H23" s="20" t="str">
         <f>ROUND(6.0, 2)</f>
       </c>
-      <c r="H23" s="20" t="str">
+      <c r="I23" s="20" t="str">
         <f>ROUND(14.7, 2)</f>
       </c>
-      <c r="I23" s="20" t="str">
+      <c r="J23" s="20" t="str">
         <f>ROUND(14.13, 2)</f>
       </c>
-      <c r="J23" s="20" t="str">
+      <c r="K23" s="20" t="str">
         <f>ROUND(14.0, 2)</f>
       </c>
-      <c r="K23" s="20" t="str">
+      <c r="L23" s="20" t="str">
         <f>ROUND(23.8, 2)</f>
       </c>
-      <c r="L23" s="20" t="str">
+      <c r="M23" s="20" t="str">
         <f>ROUND(12.0, 2)</f>
       </c>
-      <c r="M23" s="20" t="str">
+      <c r="N23" s="20" t="str">
         <f>ROUND(18.1, 2)</f>
       </c>
-      <c r="N23" s="20" t="str">
+      <c r="O23" s="20" t="str">
         <f>ROUND(5.9, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="24">
       <c r="A24" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C24" s="23" t="inlineStr">
         <is>
@@ -3842,45 +4006,48 @@
         </is>
       </c>
       <c r="D24" s="20" t="str">
+        <f>ROUND(6.3, 2)</f>
+      </c>
+      <c r="E24" s="20" t="str">
         <f>ROUND(9.0, 2)</f>
       </c>
-      <c r="E24" s="20" t="str">
+      <c r="F24" s="20" t="str">
         <f>ROUND(10.6, 2)</f>
       </c>
-      <c r="F24" s="20" t="str">
+      <c r="G24" s="20" t="str">
         <f>ROUND(19.0, 2)</f>
       </c>
-      <c r="G24" s="20" t="str">
+      <c r="H24" s="20" t="str">
         <f>ROUND(6.0, 2)</f>
       </c>
-      <c r="H24" s="20" t="str">
+      <c r="I24" s="20" t="str">
         <f>ROUND(14.1, 2)</f>
       </c>
-      <c r="I24" s="20" t="str">
+      <c r="J24" s="20" t="str">
         <f>ROUND(15.0, 2)</f>
       </c>
-      <c r="J24" s="20" t="str">
+      <c r="K24" s="20" t="str">
         <f>ROUND(13.0, 2)</f>
       </c>
-      <c r="K24" s="20" t="str">
+      <c r="L24" s="20" t="str">
         <f>ROUND(23.0, 2)</f>
       </c>
-      <c r="L24" s="20" t="str">
+      <c r="M24" s="20" t="str">
         <f>ROUND(13.0, 2)</f>
       </c>
-      <c r="M24" s="20" t="str">
+      <c r="N24" s="20" t="str">
         <f>ROUND(17.65, 2)</f>
       </c>
-      <c r="N24" s="20" t="str">
+      <c r="O24" s="20" t="str">
         <f>ROUND(6.0, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="25">
       <c r="A25" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C25" s="23" t="inlineStr">
         <is>
@@ -3888,89 +4055,95 @@
         </is>
       </c>
       <c r="D25" s="20" t="str">
+        <f>ROUND(6.3, 2)</f>
+      </c>
+      <c r="E25" s="20" t="str">
         <f>ROUND(7.0, 2)</f>
       </c>
-      <c r="E25" s="20" t="str">
+      <c r="F25" s="20" t="str">
         <f>ROUND(9.45, 2)</f>
       </c>
-      <c r="F25" s="20" t="str">
+      <c r="G25" s="20" t="str">
         <f>ROUND(19.8, 2)</f>
       </c>
-      <c r="G25" s="20" t="str">
+      <c r="H25" s="20" t="str">
         <f>ROUND(4.0, 2)</f>
       </c>
-      <c r="H25" s="20" t="str">
+      <c r="I25" s="20" t="str">
         <f>ROUND(14.51, 2)</f>
       </c>
-      <c r="I25" s="20" t="str">
+      <c r="J25" s="20" t="str">
         <f>ROUND(14.13, 2)</f>
       </c>
-      <c r="J25" s="20" t="str">
+      <c r="K25" s="20" t="str">
         <f>ROUND(11.0, 2)</f>
       </c>
-      <c r="K25" s="20" t="str">
+      <c r="L25" s="20" t="str">
         <f>ROUND(23.5, 2)</f>
       </c>
-      <c r="L25" s="20" t="str">
+      <c r="M25" s="20" t="str">
         <f>ROUND(15.0, 2)</f>
       </c>
-      <c r="M25" s="20" t="str">
+      <c r="N25" s="20" t="str">
         <f>ROUND(17.765, 2)</f>
       </c>
-      <c r="N25" s="20" t="str">
+      <c r="O25" s="20" t="str">
         <f>ROUND(5.31, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="26">
       <c r="A26" s="18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C26" s="23" t="n">
         <v>20610517</v>
       </c>
       <c r="D26" s="20" t="str">
+        <f>ROUND(7.0, 2)</f>
+      </c>
+      <c r="E26" s="20" t="str">
         <f>ROUND(10.0, 2)</f>
       </c>
-      <c r="E26" s="20" t="str">
+      <c r="F26" s="20" t="str">
         <f>ROUND(11.0, 2)</f>
       </c>
-      <c r="F26" s="20" t="str">
+      <c r="G26" s="20" t="str">
         <f>ROUND(19.9, 2)</f>
       </c>
-      <c r="G26" s="20" t="str">
+      <c r="H26" s="20" t="str">
         <f>ROUND(6.0, 2)</f>
       </c>
-      <c r="H26" s="20" t="str">
+      <c r="I26" s="20" t="str">
         <f>ROUND(14.9, 2)</f>
       </c>
-      <c r="I26" s="20" t="str">
+      <c r="J26" s="20" t="str">
         <f>ROUND(15.8, 2)</f>
       </c>
-      <c r="J26" s="20" t="str">
+      <c r="K26" s="20" t="str">
         <f>ROUND(15.0, 2)</f>
       </c>
-      <c r="K26" s="20" t="str">
+      <c r="L26" s="20" t="str">
         <f>ROUND(23.4, 2)</f>
       </c>
-      <c r="L26" s="20" t="str">
+      <c r="M26" s="20" t="str">
         <f>ROUND(12.0, 2)</f>
       </c>
-      <c r="M26" s="20" t="str">
+      <c r="N26" s="20" t="str">
         <f>ROUND(18.85, 2)</f>
       </c>
-      <c r="N26" s="20" t="str">
+      <c r="O26" s="20" t="str">
         <f>ROUND(5.22, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="27">
       <c r="A27" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C27" s="23" t="inlineStr">
         <is>
@@ -3981,42 +4154,45 @@
         <f>ROUND(7.0, 2)</f>
       </c>
       <c r="E27" s="20" t="str">
+        <f>ROUND(7.0, 2)</f>
+      </c>
+      <c r="F27" s="20" t="str">
         <f>ROUND(10.6, 2)</f>
       </c>
-      <c r="F27" s="20" t="str">
+      <c r="G27" s="20" t="str">
         <f>ROUND(19.7, 2)</f>
       </c>
-      <c r="G27" s="20" t="str">
+      <c r="H27" s="20" t="str">
         <f>ROUND(4.0, 2)</f>
       </c>
-      <c r="H27" s="20" t="str">
+      <c r="I27" s="20" t="str">
         <f>ROUND(14.5, 2)</f>
       </c>
-      <c r="I27" s="20" t="str">
+      <c r="J27" s="20" t="str">
         <f>ROUND(15.8, 2)</f>
       </c>
-      <c r="J27" s="20" t="str">
+      <c r="K27" s="20" t="str">
         <f>ROUND(15.0, 2)</f>
       </c>
-      <c r="K27" s="20" t="str">
+      <c r="L27" s="20" t="str">
         <f>ROUND(23.5, 2)</f>
       </c>
-      <c r="L27" s="20" t="str">
+      <c r="M27" s="20" t="str">
         <f>ROUND(12.0, 2)</f>
       </c>
-      <c r="M27" s="20" t="str">
+      <c r="N27" s="20" t="str">
         <f>ROUND(18.55, 2)</f>
       </c>
-      <c r="N27" s="20" t="str">
+      <c r="O27" s="20" t="str">
         <f>ROUND(6.0, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="28">
       <c r="A28" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C28" s="23" t="inlineStr">
         <is>
@@ -4024,7 +4200,7 @@
         </is>
       </c>
       <c r="D28" s="20" t="str">
-        <f>ROUND(0.0, 2)</f>
+        <f>ROUND(6.3, 2)</f>
       </c>
       <c r="E28" s="20" t="str">
         <f>ROUND(0.0, 2)</f>
@@ -4033,36 +4209,39 @@
         <f>ROUND(0.0, 2)</f>
       </c>
       <c r="G28" s="20" t="str">
+        <f>ROUND(0.0, 2)</f>
+      </c>
+      <c r="H28" s="20" t="str">
         <f>ROUND(5.0, 2)</f>
       </c>
-      <c r="H28" s="20" t="str">
+      <c r="I28" s="20" t="str">
         <f>ROUND(14.6, 2)</f>
       </c>
-      <c r="I28" s="20" t="str">
+      <c r="J28" s="20" t="str">
         <f>ROUND(15.3, 2)</f>
       </c>
-      <c r="J28" s="20" t="str">
+      <c r="K28" s="20" t="str">
         <f>ROUND(13.0, 2)</f>
       </c>
-      <c r="K28" s="20" t="str">
+      <c r="L28" s="20" t="str">
         <f>ROUND(20.88, 2)</f>
       </c>
-      <c r="L28" s="20" t="str">
+      <c r="M28" s="20" t="str">
         <f>ROUND(16.0, 2)</f>
       </c>
-      <c r="M28" s="20" t="str">
+      <c r="N28" s="20" t="str">
         <f>ROUND(17.5, 2)</f>
       </c>
-      <c r="N28" s="20" t="str">
+      <c r="O28" s="20" t="str">
         <f>ROUND(6.0, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="29">
       <c r="A29" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C29" s="23" t="inlineStr">
         <is>
@@ -4070,42 +4249,45 @@
         </is>
       </c>
       <c r="D29" s="20" t="str">
+        <f>ROUND(7.0, 2)</f>
+      </c>
+      <c r="E29" s="20" t="str">
         <f>ROUND(9.0, 2)</f>
       </c>
-      <c r="E29" s="20" t="str">
+      <c r="F29" s="20" t="str">
         <f>ROUND(10.4, 2)</f>
       </c>
-      <c r="F29" s="20" t="str">
+      <c r="G29" s="20" t="str">
         <f>ROUND(19.5, 2)</f>
       </c>
-      <c r="G29" s="20" t="str">
+      <c r="H29" s="20" t="str">
         <f>ROUND(7.0, 2)</f>
       </c>
-      <c r="H29" s="20" t="str">
+      <c r="I29" s="20" t="str">
         <f>ROUND(14.4, 2)</f>
       </c>
-      <c r="I29" s="20" t="str">
+      <c r="J29" s="20" t="str">
         <f>ROUND(15.8, 2)</f>
       </c>
-      <c r="J29" s="20" t="str">
+      <c r="K29" s="20" t="str">
         <f>ROUND(14.0, 2)</f>
       </c>
-      <c r="K29" s="20" t="str">
+      <c r="L29" s="20" t="str">
         <f>ROUND(21.24, 2)</f>
       </c>
-      <c r="L29" s="20" t="str">
+      <c r="M29" s="20" t="str">
         <f>ROUND(14.0, 2)</f>
       </c>
-      <c r="M29" s="20" t="str">
+      <c r="N29" s="20" t="str">
         <f>ROUND(18.7, 2)</f>
       </c>
-      <c r="N29" s="20" t="str">
+      <c r="O29" s="20" t="str">
         <f>ROUND(5.9, 2)</f>
       </c>
     </row>
     <row customHeight="1" ht="15" r="30">
       <c r="A30" s="28" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B30" s="29" t="inlineStr">
         <is>
@@ -4150,10 +4332,13 @@
       <c r="N30" s="33" t="str">
         <f>IFERROR(AVERAGE(N11:N29),"")</f>
       </c>
+      <c r="O30" s="33" t="str">
+        <f>IFERROR(AVERAGE(O11:O29),"")</f>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="31">
       <c r="A31" s="47" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B31" s="48" t="inlineStr">
         <is>
@@ -4198,10 +4383,13 @@
       <c r="N31" s="32" t="str">
         <f>IFERROR(MIN(N11:N29),"")</f>
       </c>
+      <c r="O31" s="32" t="str">
+        <f>IFERROR(MIN(O11:O29),"")</f>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="32">
       <c r="A32" s="47" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B32" s="48" t="inlineStr">
         <is>
@@ -4246,10 +4434,13 @@
       <c r="N32" s="32" t="str">
         <f>IFERROR(MAX(N11:N29),"")</f>
       </c>
+      <c r="O32" s="32" t="str">
+        <f>IFERROR(MAX(O11:O29),"")</f>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="33">
       <c r="A33" s="43" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B33" s="45" t="inlineStr">
         <is>
@@ -4262,36 +4453,39 @@
         </is>
       </c>
       <c r="D33" s="44" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="E33" s="44" t="n">
         <v>10.0</v>
       </c>
-      <c r="E33" s="44" t="n">
+      <c r="F33" s="44" t="n">
         <v>12.0</v>
       </c>
-      <c r="F33" s="44" t="n">
+      <c r="G33" s="44" t="n">
         <v>21.0</v>
       </c>
-      <c r="G33" s="44" t="n">
+      <c r="H33" s="44" t="n">
         <v>11.0</v>
       </c>
-      <c r="H33" s="44" t="n">
+      <c r="I33" s="44" t="n">
         <v>15.0</v>
-      </c>
-      <c r="I33" s="44" t="n">
-        <v>16.0</v>
       </c>
       <c r="J33" s="44" t="n">
         <v>16.0</v>
       </c>
       <c r="K33" s="44" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="L33" s="44" t="n">
         <v>24.0</v>
       </c>
-      <c r="L33" s="44" t="n">
+      <c r="M33" s="44" t="n">
         <v>16.0</v>
       </c>
-      <c r="M33" s="44" t="n">
+      <c r="N33" s="44" t="n">
         <v>19.0</v>
       </c>
-      <c r="N33" s="44" t="n">
+      <c r="O33" s="44" t="n">
         <v>6.0</v>
       </c>
     </row>
@@ -4302,7 +4496,7 @@
     <row customHeight="1" ht="15" r="38"/>
     <row customHeight="1" ht="15" r="39">
       <c r="A39" s="50" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B39" s="50" t="inlineStr">
         <is>
@@ -4365,6 +4559,11 @@
         </is>
       </c>
       <c r="N39" s="50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="O39" s="50" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4441,10 +4640,15 @@
           <t/>
         </is>
       </c>
+      <c r="O40" s="51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
@@ -4456,6 +4660,7 @@
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A32:C32"/>

</xml_diff>